<commit_message>
updating data, results and figures
</commit_message>
<xml_diff>
--- a/output/gamma.xlsx
+++ b/output/gamma.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t xml:space="preserve">document</t>
   </si>
@@ -32,9 +32,6 @@
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
     <t xml:space="preserve">authors</t>
   </si>
   <si>
@@ -192,6 +189,114 @@
   </si>
   <si>
     <t xml:space="preserve">VENTURA, K., FAGUNDES, V., D’ELÍA, G., CHRISTOFF, A.U., YONENAGA-YASSUDA, Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE FREITAS, T.R.O.; MATTEVI, M.S.; OLIVEIRA, L.F.B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jardim, M.M.,  Diego Queirolo, Felipe B. Peters, Fábio D. Mazim, Marina O. Favarini,
+Flávia P. Tirellia
+, Rhaysa A. Trindade, Sandro L. Bonatto, Júlio César Bicca-Marques
+and Italo Mourthe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prates, H.M.; Gabriela Pacheco Hass; Júlio César Bicca-Marques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almeida, M.A.B., Cardoso, J.C., Santos, E., Romano, A.P.M., Chiang, J.O., Martins, L.C., Vasconcelos, P.F.C. &amp; Bicca-Marques, J.C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus, A.S. &amp; Bicca-Marques, J.C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oliveira, S.G., Prates, H.M., Mentz, M. &amp; Bicca-Marques, J.C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prates, H.M. &amp; Bicca-Marques, J.C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicca-Marques, J.C., Muhle, C.B., Prates, H.M., Oliveira, S.G. &amp; Calegaro-Marques, C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicca-Marques, J.C., Prates, H.M., Aguiar, F.R.C. &amp; Jones, C.B. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicca-Marques, J.C. &amp; Calegaro-Marques, C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calegaro-Marques, C. &amp; Bicca-Marques, J.C. (1997) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calegaro-Marques, C. &amp; Bicca-Marques, J.C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicca-Marques, J.C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calegaro-Marques, C. &amp; Bicca-Marques, J.C. (1993) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santos, Maria de Fátima M. dos, Pellanda, Mateus, Tomazzoni, Ana Cristina, Hasenack, Heinrich, Hartz, Sandra Maria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROCHA-MENDES, FABIANA, KUCZACH, ANGELA MÁRCIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dias, Michele, Mikich, Sandra Bos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grazzini, Guilherme, Mochi-Junior, Cássio Marcelo, de Oliveira, Heloisa, Pontes, Jaqueline dos Santos, Gatto-Almeida, Fernanda, Tiepolo, Liliani Marilia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tortato, Fernando Rodrigo, Testoni, André Filipe, Althoff, Sérgio Luiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penter, Camila, Pedó, Ezequiel, Fabián, Marta Elena, Hartz, Sandra Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braga, Fernanda G., Kuniyoshi, Yoshiko S.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braga, Fernanda Góss, Moura-Britto, Mauro de, Margarido, Tereza Cristina Castellano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miranda, João M. D., Passos, Fernando C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miranda, João M. D., Pulchério-Leite, Atenisi, Moro-Rios,Rodrigo F., Passos, Fernando C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocha, Vlamir J., Aguiar, Lucas M., Silva-Pereira,  José E., Moro-Rios, Rodrigo F., Passos, Fernando C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dall'Agnol, B.,U. A. Souza,B. Weck,T. C. Trigo,M. M. A. Jardim,F. B. Costa,M. B. Labruna,F. B. Peters,M. O. Favarini,F. D. Mazim,C. A. S. Ferreira,J. Reck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dos Santos, M. de FM; Hartz, S. M. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linck, P., Tirelli, F. P., Bastos, M. C., Fonseca, A. N., Cardoso, L. F., &amp; Trigo, T. C. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Padilha, T. C., Zitelli, L. C., Webster, A., Dall'Agnol, B., da Rosa, V. B., Souza, U., ... &amp; Reck, J. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oliveira, S. V. D., Corrêa, L. L., Peters, F. B., Mazim, F. D., Garcias, F. M., Santos, J. P. D., &amp; Kasper, C. B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedó, Ezequiel, Tomazzoni, AC., Hartz,SM, Christoff, AU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pellanda, M., Castro Almeida, C. M., dos Santos, M. D. F. M., &amp; Hartz, S. M. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinto, L. C., &amp; Duarte, M. M. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silveira de Oliveira, Ê., Ludwig da Fontoura Rodrigues, M., Machado Severo, M., Gomes dos Santos, T., &amp; Kasper, C. B. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vieira, E. M., &amp; Port, D. </t>
   </si>
 </sst>
 </file>
@@ -545,34 +650,28 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.999453567011299</v>
+        <v>0.000141673528509361</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000109286597740139</v>
+        <v>0.000141673528509279</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000109286597740218</v>
+        <v>0.999433305885963</v>
       </c>
       <c r="E2" t="n">
-        <v>0.000109286597740255</v>
+        <v>0.000141673528509327</v>
       </c>
       <c r="F2" t="n">
-        <v>0.000109286597740129</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.000109286597740229</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
+        <v>0.00014167352850939</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -580,25 +679,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.000110167358698251</v>
+        <v>0.477673388832125</v>
       </c>
       <c r="C3" t="n">
-        <v>0.000110167358698745</v>
+        <v>0.521898397219545</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000110167358698691</v>
+        <v>0.000142737982776669</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000110167358698725</v>
+        <v>0.000142737982776603</v>
       </c>
       <c r="F3" t="n">
-        <v>0.999449163206507</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.00011016735869864</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
+        <v>0.000142737982776802</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -606,25 +702,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.999556411955849</v>
+        <v>0.99953690943639</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0000887176088303118</v>
+        <v>0.000115772640902533</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000887176088303458</v>
+        <v>0.000115772640902571</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0000887176088303341</v>
+        <v>0.000115772640902578</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000088717608830308</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.000088717608830243</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
+        <v>0.000115772640902598</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -632,25 +725,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0000929399010395358</v>
+        <v>0.99951627457098</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0000929399010395135</v>
+        <v>0.000120931357255072</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0000929399010395178</v>
+        <v>0.000120931357255112</v>
       </c>
       <c r="E5" t="n">
-        <v>0.999535300494802</v>
+        <v>0.000120931357255024</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0000929399010395239</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0000929399010394991</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
+        <v>0.000120931357255067</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -658,25 +748,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0000776330732919772</v>
+        <v>0.000101540454560227</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0000776330732918381</v>
+        <v>0.999593838181759</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0000776330732919244</v>
+        <v>0.00010154045456029</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0000776330732917012</v>
+        <v>0.000101540454560306</v>
       </c>
       <c r="F6" t="n">
-        <v>0.999611834633541</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.0000776330732918704</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
+        <v>0.000101540454560373</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -684,25 +771,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0000898843162368629</v>
+        <v>0.999539714431064</v>
       </c>
       <c r="C7" t="n">
-        <v>0.999550578418816</v>
+        <v>0.000115071392234167</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0000898843162367964</v>
+        <v>0.000115071392233852</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000089884316236656</v>
+        <v>0.000115071392234139</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0000898843162368797</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.0000898843162368285</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
+        <v>0.000115071392234134</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -710,25 +794,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0000904792534569088</v>
+        <v>0.000118665239651801</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0000904792534569127</v>
+        <v>0.999525339041393</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0000904792534568102</v>
+        <v>0.00011866523965191</v>
       </c>
       <c r="E8" t="n">
-        <v>0.999547603732716</v>
+        <v>0.000118665239651707</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0000904792534568956</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0000904792534568841</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
+        <v>0.000118665239651743</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -736,25 +817,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0000859291853007366</v>
+        <v>0.000114378587512966</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0000859291853007884</v>
+        <v>0.000114378587512898</v>
       </c>
       <c r="D9" t="n">
-        <v>0.999570354073496</v>
+        <v>0.000114378587512951</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00008592918530068</v>
+        <v>0.000114378587512975</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0000859291853006536</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.0000859291853007081</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
+        <v>0.999542485649948</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -762,25 +840,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.000130086844835125</v>
+        <v>0.986292282007555</v>
       </c>
       <c r="C10" t="n">
-        <v>0.000130086844835239</v>
+        <v>0.000167980123848391</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000130086844835166</v>
+        <v>0.0132037776208996</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000130086844835124</v>
+        <v>0.000167980123848419</v>
       </c>
       <c r="F10" t="n">
-        <v>0.999349565775824</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.000130086844835206</v>
-      </c>
-      <c r="H10" t="s">
-        <v>16</v>
+        <v>0.000167980123848449</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -788,25 +863,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.000106726833329342</v>
+        <v>0.711519614685815</v>
       </c>
       <c r="C11" t="n">
-        <v>0.000106726833329259</v>
+        <v>0.288079293543592</v>
       </c>
       <c r="D11" t="n">
-        <v>0.999466365833354</v>
+        <v>0.000133697256864384</v>
       </c>
       <c r="E11" t="n">
-        <v>0.000106726833329144</v>
+        <v>0.000133697256864316</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00010672683332934</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.000106726833329294</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
+        <v>0.000133697256864322</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -814,25 +886,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.000112896930600171</v>
+        <v>0.000144915609615739</v>
       </c>
       <c r="C12" t="n">
-        <v>0.999435515346999</v>
+        <v>0.6819095712112</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00011289693060018</v>
+        <v>0.155066976488115</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000112896930600279</v>
+        <v>0.162733621081454</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000112896930600231</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.000112896930600228</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
+        <v>0.000144915609615842</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -840,25 +909,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.000257522012022198</v>
+        <v>0.000287430417947196</v>
       </c>
       <c r="C13" t="n">
-        <v>0.000257522012022298</v>
+        <v>0.998850278328211</v>
       </c>
       <c r="D13" t="n">
-        <v>0.998712389939889</v>
+        <v>0.000287430417947299</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000257522012022293</v>
+        <v>0.000287430417947209</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00025752201202228</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.000257522012022226</v>
-      </c>
-      <c r="H13" t="s">
-        <v>19</v>
+        <v>0.000287430417947273</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -866,25 +932,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0000808470845576728</v>
+        <v>0.000102637625859775</v>
       </c>
       <c r="C14" t="n">
-        <v>0.000080847084557623</v>
+        <v>0.000102637625859628</v>
       </c>
       <c r="D14" t="n">
-        <v>0.999595764577212</v>
+        <v>0.000102637625859821</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0000808470845576186</v>
+        <v>0.000102637625859721</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0000808470845576829</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.0000808470845576765</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
+        <v>0.999589449496561</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -892,25 +955,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.000111972167627038</v>
+        <v>0.00013658083861515</v>
       </c>
       <c r="C15" t="n">
-        <v>0.000111972167627037</v>
+        <v>0.000136580838615124</v>
       </c>
       <c r="D15" t="n">
-        <v>0.000111972167627061</v>
+        <v>0.000136580838615124</v>
       </c>
       <c r="E15" t="n">
-        <v>0.000111972167627017</v>
+        <v>0.99945367664554</v>
       </c>
       <c r="F15" t="n">
-        <v>0.999440139161865</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.000111972167627003</v>
-      </c>
-      <c r="H15" t="s">
-        <v>21</v>
+        <v>0.000136580838615086</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -918,25 +978,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.000101196209487688</v>
+        <v>0.999476268329508</v>
       </c>
       <c r="C16" t="n">
-        <v>0.000101196209488082</v>
+        <v>0.000130932917622954</v>
       </c>
       <c r="D16" t="n">
-        <v>0.000101196209488064</v>
+        <v>0.000130932917622873</v>
       </c>
       <c r="E16" t="n">
-        <v>0.000101196209487823</v>
+        <v>0.000130932917623036</v>
       </c>
       <c r="F16" t="n">
-        <v>0.99949401895256</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.000101196209487931</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
+        <v>0.000130932917623048</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -944,25 +1001,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0000975841752525218</v>
+        <v>0.000120166428787889</v>
       </c>
       <c r="C17" t="n">
-        <v>0.999512079123737</v>
+        <v>0.000120166428787951</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0000975841752525272</v>
+        <v>0.000120166428787941</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0000975841752524984</v>
+        <v>0.999519334284848</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0000975841752525441</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.000097584175252516</v>
-      </c>
-      <c r="H17" t="s">
-        <v>23</v>
+        <v>0.000120166428787929</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18">
@@ -970,25 +1024,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0000887176088300816</v>
+        <v>0.521679963383764</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0000887176088301572</v>
+        <v>0.477966250747023</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0000887176088302078</v>
+        <v>0.00011792862307086</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0000887176088300402</v>
+        <v>0.000117928623070958</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0000887176088301933</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.999556411955849</v>
-      </c>
-      <c r="H18" t="s">
-        <v>24</v>
+        <v>0.000117928623071039</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19">
@@ -996,25 +1047,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.999435515346999</v>
+        <v>0.00014491560961572</v>
       </c>
       <c r="C19" t="n">
-        <v>0.000112896930600217</v>
+        <v>0.272330506796583</v>
       </c>
       <c r="D19" t="n">
-        <v>0.000112896930600178</v>
+        <v>0.000144915609615849</v>
       </c>
       <c r="E19" t="n">
-        <v>0.000112896930600205</v>
+        <v>0.72723474637457</v>
       </c>
       <c r="F19" t="n">
-        <v>0.000112896930600095</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.000112896930600153</v>
-      </c>
-      <c r="H19" t="s">
-        <v>25</v>
+        <v>0.000144915609615744</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20">
@@ -1022,25 +1070,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.999538438617237</v>
+        <v>0.000117928623070897</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0000923122765525308</v>
+        <v>0.000117928623070948</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0000923122765526098</v>
+        <v>0.000117928623070799</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0000923122765525592</v>
+        <v>0.999528285507716</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0000923122765524932</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.0000923122765525428</v>
-      </c>
-      <c r="H20" t="s">
-        <v>26</v>
+        <v>0.000117928623071008</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -1048,25 +1093,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0000715388520400753</v>
+        <v>0.999606458762582</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0000715388520400493</v>
+        <v>0.0000983853093544732</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0000715388520400295</v>
+        <v>0.0000983853093543926</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9996423057398</v>
+        <v>0.0000983853093544787</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0000715388520400206</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.0000715388520400845</v>
-      </c>
-      <c r="H21" t="s">
-        <v>27</v>
+        <v>0.000098385309354467</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22">
@@ -1074,25 +1116,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.999482526524166</v>
+        <v>0.999483389329016</v>
       </c>
       <c r="C22" t="n">
-        <v>0.000103494695166737</v>
+        <v>0.000129152667745992</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000103494695166789</v>
+        <v>0.000129152667746053</v>
       </c>
       <c r="E22" t="n">
-        <v>0.000103494695166753</v>
+        <v>0.000129152667746087</v>
       </c>
       <c r="F22" t="n">
-        <v>0.000103494695166514</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.000103494695166787</v>
-      </c>
-      <c r="H22" t="s">
-        <v>28</v>
+        <v>0.000129152667746102</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23">
@@ -1100,25 +1139,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.000143768384896564</v>
+        <v>0.000172557447286849</v>
       </c>
       <c r="C23" t="n">
-        <v>0.000143768384896604</v>
+        <v>0.000172557447286801</v>
       </c>
       <c r="D23" t="n">
-        <v>0.999281158075517</v>
+        <v>0.999309770210853</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00014376838489661</v>
+        <v>0.000172557447286852</v>
       </c>
       <c r="F23" t="n">
-        <v>0.000143768384896617</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.000143768384896576</v>
-      </c>
-      <c r="H23" t="s">
-        <v>29</v>
+        <v>0.000172557447286845</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24">
@@ -1126,25 +1162,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.000160666007572058</v>
+        <v>0.000193666470265886</v>
       </c>
       <c r="C24" t="n">
-        <v>0.99919666996214</v>
+        <v>0.000193666470265835</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000160666007572267</v>
+        <v>0.999225334118937</v>
       </c>
       <c r="E24" t="n">
-        <v>0.00016066600757212</v>
+        <v>0.00019366647026594</v>
       </c>
       <c r="F24" t="n">
-        <v>0.000160666007571995</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.000160666007572073</v>
-      </c>
-      <c r="H24" t="s">
-        <v>30</v>
+        <v>0.000193666470265788</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25">
@@ -1152,25 +1185,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.000133909854405082</v>
+        <v>0.987957202874711</v>
       </c>
       <c r="C25" t="n">
-        <v>0.00013390985440509</v>
+        <v>0.000158189033636265</v>
       </c>
       <c r="D25" t="n">
-        <v>0.000133909854405096</v>
+        <v>0.000158189033636204</v>
       </c>
       <c r="E25" t="n">
-        <v>0.999330450727975</v>
+        <v>0.000158189033636253</v>
       </c>
       <c r="F25" t="n">
-        <v>0.000133909854405057</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.000133909854404984</v>
-      </c>
-      <c r="H25" t="s">
-        <v>31</v>
+        <v>0.0115682300243798</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26">
@@ -1178,25 +1208,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.000108419808019863</v>
+        <v>0.000136580838614994</v>
       </c>
       <c r="C26" t="n">
-        <v>0.999457900959901</v>
+        <v>0.000136580838615045</v>
       </c>
       <c r="D26" t="n">
-        <v>0.000108419808020017</v>
+        <v>0.000136580838615091</v>
       </c>
       <c r="E26" t="n">
-        <v>0.000108419808019728</v>
+        <v>0.99945367664554</v>
       </c>
       <c r="F26" t="n">
-        <v>0.000108419808019978</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.000108419808019908</v>
-      </c>
-      <c r="H26" t="s">
-        <v>32</v>
+        <v>0.000136580838615033</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27">
@@ -1204,25 +1231,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.999575688572405</v>
+        <v>0.00011168882954902</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0000848622855190582</v>
+        <v>0.000111688829549008</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0000848622855190231</v>
+        <v>0.999553244681804</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0000848622855190705</v>
+        <v>0.000111688829548892</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0000848622855190097</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.0000848622855190129</v>
-      </c>
-      <c r="H27" t="s">
-        <v>33</v>
+        <v>0.000111688829549066</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28">
@@ -1230,25 +1254,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0000916930719204547</v>
+        <v>0.999534070044648</v>
       </c>
       <c r="C28" t="n">
-        <v>0.000091693071920467</v>
+        <v>0.000116482488838206</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0000916930719203895</v>
+        <v>0.000116482488838063</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0000916930719203981</v>
+        <v>0.000116482488837917</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0000916930719203117</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.999541534640398</v>
-      </c>
-      <c r="H28" t="s">
-        <v>34</v>
+        <v>0.000116482488838192</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29">
@@ -1256,25 +1277,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.000137964369728569</v>
+        <v>0.000162241872333957</v>
       </c>
       <c r="C29" t="n">
-        <v>0.00013796436972853</v>
+        <v>0.586269180668495</v>
       </c>
       <c r="D29" t="n">
-        <v>0.000137964369728585</v>
+        <v>0.413244093714503</v>
       </c>
       <c r="E29" t="n">
-        <v>0.000137964369728627</v>
+        <v>0.000162241872333974</v>
       </c>
       <c r="F29" t="n">
-        <v>0.999310178151357</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.000137964369728544</v>
-      </c>
-      <c r="H29" t="s">
-        <v>35</v>
+        <v>0.000162241872333969</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30">
@@ -1282,25 +1300,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.000104284236678128</v>
+        <v>0.000134644826003831</v>
       </c>
       <c r="C30" t="n">
-        <v>0.000104284236678067</v>
+        <v>0.000134644826003759</v>
       </c>
       <c r="D30" t="n">
-        <v>0.99947857881661</v>
+        <v>0.000134644826003805</v>
       </c>
       <c r="E30" t="n">
-        <v>0.000104284236677997</v>
+        <v>0.000134644826003782</v>
       </c>
       <c r="F30" t="n">
-        <v>0.000104284236678064</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.000104284236678064</v>
-      </c>
-      <c r="H30" t="s">
-        <v>36</v>
+        <v>0.999461420695985</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="31">
@@ -1308,25 +1323,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.000162576832383334</v>
+        <v>0.000201899277272789</v>
       </c>
       <c r="C31" t="n">
-        <v>0.000162576832383361</v>
+        <v>0.000201899277272744</v>
       </c>
       <c r="D31" t="n">
-        <v>0.999187115838083</v>
+        <v>0.0519201415312905</v>
       </c>
       <c r="E31" t="n">
-        <v>0.000162576832383456</v>
+        <v>0.000201899277272732</v>
       </c>
       <c r="F31" t="n">
-        <v>0.000162576832383325</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.000162576832383322</v>
-      </c>
-      <c r="H31" t="s">
-        <v>37</v>
+        <v>0.947474160636891</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="32">
@@ -1334,25 +1346,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0000942211060000736</v>
+        <v>0.999510036775245</v>
       </c>
       <c r="C32" t="n">
-        <v>0.000094221106000122</v>
+        <v>0.000122490806188733</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0000942211060001315</v>
+        <v>0.000122490806188688</v>
       </c>
       <c r="E32" t="n">
-        <v>0.99952889447</v>
+        <v>0.000122490806188747</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0000942211059997171</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.0000942211060001821</v>
-      </c>
-      <c r="H32" t="s">
-        <v>38</v>
+        <v>0.000122490806188775</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33">
@@ -1360,25 +1369,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.999257738456756</v>
+        <v>0.000186078772847529</v>
       </c>
       <c r="C33" t="n">
-        <v>0.000148452308648909</v>
+        <v>0.000186078772847316</v>
       </c>
       <c r="D33" t="n">
-        <v>0.000148452308648844</v>
+        <v>0.99925568490861</v>
       </c>
       <c r="E33" t="n">
-        <v>0.000148452308648918</v>
+        <v>0.000186078772847335</v>
       </c>
       <c r="F33" t="n">
-        <v>0.000148452308648846</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.000148452308648894</v>
-      </c>
-      <c r="H33" t="s">
-        <v>39</v>
+        <v>0.000186078772847305</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34">
@@ -1386,25 +1392,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0000955381283180181</v>
+        <v>0.000120931357255068</v>
       </c>
       <c r="C34" t="n">
-        <v>0.999522309358409</v>
+        <v>0.000120931357255171</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0000955381283181321</v>
+        <v>0.999516274570979</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0000955381283181732</v>
+        <v>0.000120931357255154</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0000955381283180609</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.0000955381283182012</v>
-      </c>
-      <c r="H34" t="s">
-        <v>40</v>
+        <v>0.000120931357255211</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35">
@@ -1412,25 +1415,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.000121962366670207</v>
+        <v>0.999382665032685</v>
       </c>
       <c r="C35" t="n">
-        <v>0.999390188166648</v>
+        <v>0.000154333741828916</v>
       </c>
       <c r="D35" t="n">
-        <v>0.000121962366670395</v>
+        <v>0.000154333741828776</v>
       </c>
       <c r="E35" t="n">
-        <v>0.000121962366670352</v>
+        <v>0.000154333741828821</v>
       </c>
       <c r="F35" t="n">
-        <v>0.000121962366670321</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.000121962366670202</v>
-      </c>
-      <c r="H35" t="s">
-        <v>41</v>
+        <v>0.00015433374182877</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="36">
@@ -1438,25 +1438,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.000203777234560514</v>
+        <v>0.000243264139427258</v>
       </c>
       <c r="C36" t="n">
-        <v>0.000203777234560416</v>
+        <v>0.000243264139427296</v>
       </c>
       <c r="D36" t="n">
-        <v>0.000203777234560441</v>
+        <v>0.000243264139427104</v>
       </c>
       <c r="E36" t="n">
-        <v>0.998981113827198</v>
+        <v>0.999026943442291</v>
       </c>
       <c r="F36" t="n">
-        <v>0.000203777234560503</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.000203777234560501</v>
-      </c>
-      <c r="H36" t="s">
-        <v>42</v>
+        <v>0.000243264139427214</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="37">
@@ -1464,25 +1461,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.000140806592655862</v>
+        <v>0.000180767041753228</v>
       </c>
       <c r="C37" t="n">
-        <v>0.000140806592655929</v>
+        <v>0.000180767041753158</v>
       </c>
       <c r="D37" t="n">
-        <v>0.000140806592655898</v>
+        <v>0.999276931832987</v>
       </c>
       <c r="E37" t="n">
-        <v>0.000140806592655851</v>
+        <v>0.000180767041753072</v>
       </c>
       <c r="F37" t="n">
-        <v>0.000140806592655845</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.999295967036721</v>
-      </c>
-      <c r="H37" t="s">
-        <v>43</v>
+        <v>0.000180767041753189</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38">
@@ -1490,25 +1484,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0000808470845576302</v>
+        <v>0.000104328572326761</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0000808470845576326</v>
+        <v>0.000104328572326724</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0000808470845576697</v>
+        <v>0.000104328572326806</v>
       </c>
       <c r="E38" t="n">
-        <v>0.999595764577212</v>
+        <v>0.999582685710693</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0000808470845577297</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.0000808470845575936</v>
-      </c>
-      <c r="H38" t="s">
-        <v>44</v>
+        <v>0.000104328572326904</v>
+      </c>
+      <c r="G38" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39">
@@ -1516,25 +1507,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.000111972167627066</v>
+        <v>0.999441633806337</v>
       </c>
       <c r="C39" t="n">
-        <v>0.999440139161864</v>
+        <v>0.000139591548415682</v>
       </c>
       <c r="D39" t="n">
-        <v>0.000111972167627122</v>
+        <v>0.000139591548415763</v>
       </c>
       <c r="E39" t="n">
-        <v>0.000111972167627153</v>
+        <v>0.000139591548415598</v>
       </c>
       <c r="F39" t="n">
-        <v>0.000111972167627064</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0.000111972167627131</v>
-      </c>
-      <c r="H39" t="s">
-        <v>45</v>
+        <v>0.000139591548415707</v>
+      </c>
+      <c r="G39" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="40">
@@ -1542,25 +1530,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.999538438617238</v>
+        <v>0.000115071392233927</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0000923122765521209</v>
+        <v>0.000115071392234121</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0000923122765524614</v>
+        <v>0.999539714431064</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0000923122765523911</v>
+        <v>0.000115071392234307</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0000923122765524421</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0.0000923122765523073</v>
-      </c>
-      <c r="H40" t="s">
-        <v>46</v>
+        <v>0.000115071392234101</v>
+      </c>
+      <c r="G40" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41">
@@ -1568,25 +1553,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.000140806592655835</v>
+        <v>0.000172557447286781</v>
       </c>
       <c r="C41" t="n">
-        <v>0.999295967036721</v>
+        <v>0.000172557447287016</v>
       </c>
       <c r="D41" t="n">
-        <v>0.000140806592655823</v>
+        <v>0.999309770210852</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0001408065926559</v>
+        <v>0.000172557447286966</v>
       </c>
       <c r="F41" t="n">
-        <v>0.000140806592655843</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0.000140806592655818</v>
-      </c>
-      <c r="H41" t="s">
-        <v>47</v>
+        <v>0.00017255744728684</v>
+      </c>
+      <c r="G41" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="42">
@@ -1594,25 +1576,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>0.000107566659721813</v>
+        <v>0.450637041914509</v>
       </c>
       <c r="C42" t="n">
-        <v>0.320528446003462</v>
+        <v>0.0998275801279008</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00010756665972188</v>
+        <v>0.000132762931642951</v>
       </c>
       <c r="E42" t="n">
-        <v>0.00010756665972177</v>
+        <v>0.449269852094305</v>
       </c>
       <c r="F42" t="n">
-        <v>0.000107566659721809</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0.679041287357651</v>
-      </c>
-      <c r="H42" t="s">
-        <v>48</v>
+        <v>0.000132762931643002</v>
+      </c>
+      <c r="G42" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43">
@@ -1620,25 +1599,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>0.000127657177438729</v>
+        <v>0.000156882711751835</v>
       </c>
       <c r="C43" t="n">
-        <v>0.00012765717743845</v>
+        <v>0.999372469152992</v>
       </c>
       <c r="D43" t="n">
-        <v>0.00012765717743877</v>
+        <v>0.000156882711751967</v>
       </c>
       <c r="E43" t="n">
-        <v>0.000127657177438649</v>
+        <v>0.000156882711751913</v>
       </c>
       <c r="F43" t="n">
-        <v>0.000127657177438668</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.999361714112807</v>
-      </c>
-      <c r="H43" t="s">
-        <v>49</v>
+        <v>0.000156882711751939</v>
+      </c>
+      <c r="G43" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="44">
@@ -1646,25 +1622,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>0.000220189171441044</v>
+        <v>0.638617941977231</v>
       </c>
       <c r="C44" t="n">
-        <v>0.000220189171441021</v>
+        <v>0.000263509441713748</v>
       </c>
       <c r="D44" t="n">
-        <v>0.00022018917144097</v>
+        <v>0.360591529697627</v>
       </c>
       <c r="E44" t="n">
-        <v>0.000220189171440934</v>
+        <v>0.000263509441713837</v>
       </c>
       <c r="F44" t="n">
-        <v>0.998899054142795</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0.00022018917144096</v>
-      </c>
-      <c r="H44" t="s">
-        <v>50</v>
+        <v>0.000263509441713781</v>
+      </c>
+      <c r="G44" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="45">
@@ -1672,25 +1645,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>0.000133909854405033</v>
+        <v>0.000174139164738624</v>
       </c>
       <c r="C45" t="n">
-        <v>0.000133909854404944</v>
+        <v>0.000174139164738656</v>
       </c>
       <c r="D45" t="n">
-        <v>0.000133909854404618</v>
+        <v>0.000174139164738638</v>
       </c>
       <c r="E45" t="n">
-        <v>0.000133909854405037</v>
+        <v>0.000174139164738685</v>
       </c>
       <c r="F45" t="n">
-        <v>0.00013390985440504</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.999330450727975</v>
-      </c>
-      <c r="H45" t="s">
-        <v>51</v>
+        <v>0.999303443341045</v>
+      </c>
+      <c r="G45" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46">
@@ -1698,25 +1668,22 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>0.000172855833539125</v>
+        <v>0.000210863117793581</v>
       </c>
       <c r="C46" t="n">
-        <v>0.000172855833539116</v>
+        <v>0.000210863117793591</v>
       </c>
       <c r="D46" t="n">
-        <v>0.999135720832304</v>
+        <v>0.000210863117793638</v>
       </c>
       <c r="E46" t="n">
-        <v>0.00017285583353907</v>
+        <v>0.00021086311779354</v>
       </c>
       <c r="F46" t="n">
-        <v>0.000172855833539123</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.000172855833539178</v>
-      </c>
-      <c r="H46" t="s">
-        <v>52</v>
+        <v>0.999156547528826</v>
+      </c>
+      <c r="G46" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="47">
@@ -1724,25 +1691,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>0.000126476063512859</v>
+        <v>0.000163639364804182</v>
       </c>
       <c r="C47" t="n">
-        <v>0.000126476063512969</v>
+        <v>0.000163639364804283</v>
       </c>
       <c r="D47" t="n">
-        <v>0.999367619682435</v>
+        <v>0.000163639364804231</v>
       </c>
       <c r="E47" t="n">
-        <v>0.000126476063512918</v>
+        <v>0.000163639364804306</v>
       </c>
       <c r="F47" t="n">
-        <v>0.000126476063512918</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.000126476063512965</v>
-      </c>
-      <c r="H47" t="s">
-        <v>53</v>
+        <v>0.999345442540783</v>
+      </c>
+      <c r="G47" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="48">
@@ -1750,25 +1714,22 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>0.000184522351035781</v>
+        <v>0.00023426490986545</v>
       </c>
       <c r="C48" t="n">
-        <v>0.110229065380598</v>
+        <v>0.000234264909865385</v>
       </c>
       <c r="D48" t="n">
-        <v>0.000184522351035771</v>
+        <v>0.999062940360538</v>
       </c>
       <c r="E48" t="n">
-        <v>0.000184522351035762</v>
+        <v>0.000234264909865503</v>
       </c>
       <c r="F48" t="n">
-        <v>0.000184522351035832</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.889032845215259</v>
-      </c>
-      <c r="H48" t="s">
-        <v>54</v>
+        <v>0.000234264909865384</v>
+      </c>
+      <c r="G48" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="49">
@@ -1776,25 +1737,22 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>0.000103494695166754</v>
+        <v>0.000130036699902447</v>
       </c>
       <c r="C49" t="n">
-        <v>0.000103494695166756</v>
+        <v>0.000130036699902466</v>
       </c>
       <c r="D49" t="n">
-        <v>0.999482526524166</v>
+        <v>0.000130036699902378</v>
       </c>
       <c r="E49" t="n">
-        <v>0.000103494695166771</v>
+        <v>0.000130036699902473</v>
       </c>
       <c r="F49" t="n">
-        <v>0.000103494695166717</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.000103494695166593</v>
-      </c>
-      <c r="H49" t="s">
-        <v>55</v>
+        <v>0.99947985320039</v>
+      </c>
+      <c r="G49" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="50">
@@ -1802,25 +1760,22 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>0.000145296502456455</v>
+        <v>0.000179063219129395</v>
       </c>
       <c r="C50" t="n">
-        <v>0.000145296502456515</v>
+        <v>0.000179063219129378</v>
       </c>
       <c r="D50" t="n">
-        <v>0.000145296502456557</v>
+        <v>0.000179063219129372</v>
       </c>
       <c r="E50" t="n">
-        <v>0.000145296502456482</v>
+        <v>0.000179063219129507</v>
       </c>
       <c r="F50" t="n">
-        <v>0.999273517487717</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0.000145296502456516</v>
-      </c>
-      <c r="H50" t="s">
-        <v>56</v>
+        <v>0.999283747123482</v>
+      </c>
+      <c r="G50" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="51">
@@ -1828,25 +1783,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0000955381283183494</v>
+        <v>0.00011941111631766</v>
       </c>
       <c r="C51" t="n">
-        <v>0.999522309358408</v>
+        <v>0.999522355534729</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0000955381283183771</v>
+        <v>0.000119411116317672</v>
       </c>
       <c r="E51" t="n">
-        <v>0.000095538128318319</v>
+        <v>0.000119411116317662</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0000955381283183105</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0.0000955381283183284</v>
-      </c>
-      <c r="H51" t="s">
-        <v>57</v>
+        <v>0.000119411116317749</v>
+      </c>
+      <c r="G51" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="52">
@@ -1854,25 +1806,22 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>0.000716370131439455</v>
+        <v>0.000701152176082292</v>
       </c>
       <c r="C52" t="n">
-        <v>0.000716370131439429</v>
+        <v>0.397630613067648</v>
       </c>
       <c r="D52" t="n">
-        <v>0.000716370131439398</v>
+        <v>0.000701152176082268</v>
       </c>
       <c r="E52" t="n">
-        <v>0.00071637013143944</v>
+        <v>0.000701152176082296</v>
       </c>
       <c r="F52" t="n">
-        <v>0.996418149342803</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0.000716370131439445</v>
-      </c>
-      <c r="H52" t="s">
-        <v>58</v>
+        <v>0.600265930404105</v>
+      </c>
+      <c r="G52" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="53">
@@ -1880,25 +1829,965 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0000615528818750646</v>
+        <v>0.0000815020104098802</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0000615528818750775</v>
+        <v>0.0000815020104100077</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0000615528818751685</v>
+        <v>0.0000815020104100332</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0000615528818750378</v>
+        <v>0.0000815020104099565</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0000615528818750931</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0.999692235590624</v>
-      </c>
-      <c r="H53" t="s">
+        <v>0.99967399195836</v>
+      </c>
+      <c r="G53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.0026776237970034</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.0026776237970034</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.0026776237970034</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.00267762379700338</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.989289504811986</v>
+      </c>
+      <c r="G54" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.000412142638074719</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.998351429447701</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.000412142638074761</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.000412142638074806</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.000412142638074707</v>
+      </c>
+      <c r="G55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.000154333741828714</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.00015433374182884</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.000154333741828771</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.999382665032685</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.000154333741828818</v>
+      </c>
+      <c r="G56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.00171227848467063</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.993150886061318</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.00171227848467064</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.00171227848467061</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.00171227848467064</v>
+      </c>
+      <c r="G57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.000371811614449697</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.000371811614449841</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.000371811614449687</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.998512753542201</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.000371811614449625</v>
+      </c>
+      <c r="G58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.000106076168502059</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.999575695325992</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.000106076168502088</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.000106076168502033</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.000106076168501457</v>
+      </c>
+      <c r="G59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.000059536222331778</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.0000595362223312743</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.000059536222331809</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.0000595362223317675</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.999761855110673</v>
+      </c>
+      <c r="G60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.000150661897048768</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.000150661897048864</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.000150661897048862</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.999397352411805</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.000150661897048928</v>
+      </c>
+      <c r="G61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.000100466492152875</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.999598134031388</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.000100466492153041</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.000100466492152659</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.000100466492153007</v>
+      </c>
+      <c r="G62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.000120931357255104</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.000120931357255156</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.000120931357255123</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.999516274570979</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.000120931357255132</v>
+      </c>
+      <c r="G63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.99962583596338</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.0000935410091549534</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0000935410091552162</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.0000935410091546553</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.0000935410091551701</v>
+      </c>
+      <c r="G64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.0026776237970034</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.989289504811986</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.00267762379700339</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.00267762379700338</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.00267762379700336</v>
+      </c>
+      <c r="G65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.873093391356032</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.125791173800619</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.000371811614449597</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.000371811614449722</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.000371811614449627</v>
+      </c>
+      <c r="G66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.000557199488570846</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.997771202045717</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.000557199488570825</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.000557199488570796</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.000557199488570812</v>
+      </c>
+      <c r="G67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.00038695823635235</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.000386958236352498</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.000386958236352315</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.998452167054591</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.000386958236352322</v>
+      </c>
+      <c r="G68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.000180767041753141</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.162374128291525</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.837083570583215</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.000180767041753239</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.000180767041753211</v>
+      </c>
+      <c r="G69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.00118034940648151</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.995278602374074</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.00118034940648152</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.0011803494064815</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.00118034940648152</v>
+      </c>
+      <c r="G70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0023468483079263</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.990612606768295</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.00234684830792629</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.00234684830792627</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.00234684830792627</v>
+      </c>
+      <c r="G71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.000332738663507427</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.99866904534597</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.000332738663507422</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.000332738663507413</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.00033273866350744</v>
+      </c>
+      <c r="G72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.00049869315902293</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.998005227363908</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.000498693159022927</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.000498693159022892</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.000498693159022909</v>
+      </c>
+      <c r="G73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.000104904670943121</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.000104904670943235</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.999580381316227</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.000104904670942994</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.000104904670943307</v>
+      </c>
+      <c r="G74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.597360992378247</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.000160868047124964</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.402156403480378</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.000160868047125163</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.000160868047125121</v>
+      </c>
+      <c r="G75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.000158189033636261</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.999367243865455</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.000158189033636242</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.00015818903363627</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.000158189033636358</v>
+      </c>
+      <c r="G76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.000167980123848593</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.999328079504606</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.000167980123848516</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.000167980123848666</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.000167980123848549</v>
+      </c>
+      <c r="G77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.000274950623508851</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.000274950623508914</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.00027495062350895</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.998900197505964</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.000274950623508842</v>
+      </c>
+      <c r="G78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.000139591548415794</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.000139591548415636</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.999441633806337</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.000139591548415699</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.000139591548415712</v>
+      </c>
+      <c r="G79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.999345442540783</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.000163639364804314</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.000163639364804232</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.000163639364804326</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.000163639364804292</v>
+      </c>
+      <c r="G80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.000151866277006868</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.000151866277006841</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.999392534891973</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.00015186627700684</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.000151866277006777</v>
+      </c>
+      <c r="G81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.000231411326303149</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.000231411326303229</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.000231411326303201</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.999074354694787</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.00023141132630315</v>
+      </c>
+      <c r="G82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.000512136839112977</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.000512136839113001</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.000512136839112987</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.997951452643548</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.00051213683911299</v>
+      </c>
+      <c r="G83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.000116482488838033</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.00011648248883814</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.000116482488837634</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.999534070044648</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.000116482488838154</v>
+      </c>
+      <c r="G84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.000162241872333917</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.000162241872334001</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.000162241872333895</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.999351032510664</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.000162241872333988</v>
+      </c>
+      <c r="G85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.000240188544577478</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.000240188544577499</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.99903924582169</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.000240188544577626</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.000240188544577493</v>
+      </c>
+      <c r="G86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.000120166428787629</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.999519334284849</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0001201664287879</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.000120166428787641</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.000120166428787995</v>
+      </c>
+      <c r="G87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.000115772640902516</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.000115772640902552</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.000115772640902524</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.99953690943639</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.000115772640902554</v>
+      </c>
+      <c r="G88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.000301096974890096</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.998795612100439</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.000301096974890235</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.000301096974890151</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.000301096974890152</v>
+      </c>
+      <c r="G89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.000179063219129384</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.000179063219129321</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.2200203292023</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.779442481140311</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.000179063219129393</v>
+      </c>
+      <c r="G90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.000112349338949871</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.000112349338949943</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.9995506026442</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.000112349338949821</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.000112349338949863</v>
+      </c>
+      <c r="G91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.000412142638074751</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.0456559592322562</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.95310761285352</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.000412142638074702</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.000412142638074731</v>
+      </c>
+      <c r="G92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.999461420695986</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.000134644826003565</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.000134644826003503</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.000134644826003613</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.00013464482600366</v>
+      </c>
+      <c r="G93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.000110390839055501</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.000110390839055701</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.000110390839055702</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.999558436643777</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.00011039083905567</v>
+      </c>
+      <c r="G94" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating data, results and figs
</commit_message>
<xml_diff>
--- a/output/gamma.xlsx
+++ b/output/gamma.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">document</t>
   </si>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">authors</t>
@@ -264,9 +258,6 @@
   </si>
   <si>
     <t xml:space="preserve">Miranda, João M. D., Pulchério-Leite, Atenisi, Moro-Rios,Rodrigo F., Passos, Fernando C. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rocha, Vlamir J., Aguiar, Lucas M., Silva-Pereira,  José E., Moro-Rios, Rodrigo F., Passos, Fernando C.</t>
   </si>
   <si>
     <t xml:space="preserve">Dall'Agnol, B.,U. A. Souza,B. Weck,T. C. Trigo,M. M. A. Jardim,F. B. Costa,M. B. Labruna,F. B. Peters,M. O. Favarini,F. D. Mazim,C. A. S. Ferreira,J. Reck</t>
@@ -644,34 +635,22 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.000141673528509361</v>
+        <v>0.000192407361896368</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000141673528509279</v>
+        <v>0.000192407361896298</v>
       </c>
       <c r="D2" t="n">
-        <v>0.999433305885963</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.000141673528509327</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.00014167352850939</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
+        <v>0.999615185276207</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -679,22 +658,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.477673388832125</v>
+        <v>0.999612293615071</v>
       </c>
       <c r="C3" t="n">
-        <v>0.521898397219545</v>
+        <v>0.000193853192464401</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000142737982776669</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.000142737982776603</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.000142737982776802</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
+        <v>0.000193853192464162</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -702,22 +675,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.99953690943639</v>
+        <v>0.999685545010371</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000115772640902533</v>
+        <v>0.00015722749481437</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000115772640902571</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.000115772640902578</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.000115772640902598</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
+        <v>0.000157227494814424</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -725,22 +692,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.99951627457098</v>
+        <v>0.99967153163204</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000120931357255072</v>
+        <v>0.000164234183980017</v>
       </c>
       <c r="D5" t="n">
-        <v>0.000120931357255112</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.000120931357255024</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.000120931357255067</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
+        <v>0.000164234183979945</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -748,22 +709,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.000101540454560227</v>
+        <v>0.000137897353776217</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999593838181759</v>
+        <v>0.999724205292447</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00010154045456029</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.000101540454560306</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.000101540454560373</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
+        <v>0.00013789735377651</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -771,22 +726,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.999539714431064</v>
+        <v>0.999687449904706</v>
       </c>
       <c r="C7" t="n">
-        <v>0.000115071392234167</v>
+        <v>0.000156275047647196</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000115071392233852</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.000115071392234139</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.000115071392234134</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
+        <v>0.000156275047646725</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -794,22 +743,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.000118665239651801</v>
+        <v>0.99967768743636</v>
       </c>
       <c r="C8" t="n">
-        <v>0.999525339041393</v>
+        <v>0.000161156281819906</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00011866523965191</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.000118665239651707</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.000118665239651743</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
+        <v>0.000161156281819883</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -817,22 +760,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.000114378587512966</v>
+        <v>0.000155334070398966</v>
       </c>
       <c r="C9" t="n">
-        <v>0.000114378587512898</v>
+        <v>0.000155334070399546</v>
       </c>
       <c r="D9" t="n">
-        <v>0.000114378587512951</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.000114378587512975</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.999542485649948</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
+        <v>0.999689331859202</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -840,22 +777,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.986292282007555</v>
+        <v>0.000228140009359792</v>
       </c>
       <c r="C10" t="n">
-        <v>0.000167980123848391</v>
+        <v>0.000228140009359377</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0132037776208996</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.000167980123848419</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.000167980123848449</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
+        <v>0.999543719981281</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -863,22 +794,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.711519614685815</v>
+        <v>0.999636853169583</v>
       </c>
       <c r="C11" t="n">
-        <v>0.288079293543592</v>
+        <v>0.000181573415208315</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000133697256864384</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.000133697256864316</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.000133697256864322</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
+        <v>0.000181573415208333</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -886,22 +811,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.000144915609615739</v>
+        <v>0.000196811035748827</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6819095712112</v>
+        <v>0.00019681103574884</v>
       </c>
       <c r="D12" t="n">
-        <v>0.155066976488115</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.162733621081454</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.000144915609615842</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
+        <v>0.999606377928502</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -909,22 +828,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.000287430417947196</v>
+        <v>0.000390413065926358</v>
       </c>
       <c r="C13" t="n">
-        <v>0.998850278328211</v>
+        <v>0.999219173868147</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000287430417947299</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.000287430417947209</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.000287430417947273</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
+        <v>0.000390413065926133</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14">
@@ -932,22 +845,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.000102637625859775</v>
+        <v>0.99972122497482</v>
       </c>
       <c r="C14" t="n">
-        <v>0.000102637625859628</v>
+        <v>0.000139387512589966</v>
       </c>
       <c r="D14" t="n">
-        <v>0.000102637625859821</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.000102637625859721</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.999589449496561</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
+        <v>0.000139387512589978</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -955,22 +862,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.00013658083861515</v>
+        <v>0.000185490085172385</v>
       </c>
       <c r="C15" t="n">
-        <v>0.000136580838615124</v>
+        <v>0.999629019829655</v>
       </c>
       <c r="D15" t="n">
-        <v>0.000136580838615124</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.99945367664554</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.000136580838615086</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
+        <v>0.000185490085172321</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16">
@@ -978,22 +879,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.999476268329508</v>
+        <v>0.999644362544221</v>
       </c>
       <c r="C16" t="n">
-        <v>0.000130932917622954</v>
+        <v>0.000177818727889327</v>
       </c>
       <c r="D16" t="n">
-        <v>0.000130932917622873</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.000130932917623036</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.000130932917623048</v>
-      </c>
-      <c r="G16" t="s">
-        <v>21</v>
+        <v>0.00017781872788948</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -1001,22 +896,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.000120166428787889</v>
+        <v>0.000163195236022703</v>
       </c>
       <c r="C17" t="n">
-        <v>0.000120166428787951</v>
+        <v>0.000163195236022589</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000120166428787941</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.999519334284848</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.000120166428787929</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
+        <v>0.999673609527955</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -1024,22 +913,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.521679963383764</v>
+        <v>0.263469691570063</v>
       </c>
       <c r="C18" t="n">
-        <v>0.477966250747023</v>
+        <v>0.736370152637878</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00011792862307086</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.000117928623070958</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.000117928623071039</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
+        <v>0.000160155792059275</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19">
@@ -1047,22 +930,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.00014491560961572</v>
+        <v>0.000196811035748649</v>
       </c>
       <c r="C19" t="n">
-        <v>0.272330506796583</v>
+        <v>0.999606377928503</v>
       </c>
       <c r="D19" t="n">
-        <v>0.000144915609615849</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.72723474637457</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.000144915609615744</v>
-      </c>
-      <c r="G19" t="s">
-        <v>24</v>
+        <v>0.000196811035748453</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -1070,22 +947,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.000117928623070897</v>
+        <v>0.000160155792059184</v>
       </c>
       <c r="C20" t="n">
-        <v>0.000117928623070948</v>
+        <v>0.000160155792059241</v>
       </c>
       <c r="D20" t="n">
-        <v>0.000117928623070799</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.999528285507716</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.000117928623071008</v>
-      </c>
-      <c r="G20" t="s">
-        <v>25</v>
+        <v>0.999679688415882</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21">
@@ -1093,22 +964,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.999606458762582</v>
+        <v>0.999732775784437</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0000983853093544732</v>
+        <v>0.000133612107781336</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0000983853093543926</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.0000983853093544787</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.000098385309354467</v>
-      </c>
-      <c r="G21" t="s">
-        <v>26</v>
+        <v>0.000133612107781378</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22">
@@ -1116,22 +981,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.999483389329016</v>
+        <v>0.915655056136632</v>
       </c>
       <c r="C22" t="n">
-        <v>0.000129152667745992</v>
+        <v>0.000175400698511133</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000129152667746053</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.000129152667746087</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.000129152667746102</v>
-      </c>
-      <c r="G22" t="s">
-        <v>27</v>
+        <v>0.0841695431648567</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -1139,22 +998,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.000172557447286849</v>
+        <v>0.000234357635094865</v>
       </c>
       <c r="C23" t="n">
-        <v>0.000172557447286801</v>
+        <v>0.000234357635094996</v>
       </c>
       <c r="D23" t="n">
-        <v>0.999309770210853</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.000172557447286852</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.000172557447286845</v>
-      </c>
-      <c r="G23" t="s">
-        <v>28</v>
+        <v>0.99953128472981</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24">
@@ -1162,22 +1015,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.000193666470265886</v>
+        <v>0.000263031843813452</v>
       </c>
       <c r="C24" t="n">
-        <v>0.000193666470265835</v>
+        <v>0.000263031843813557</v>
       </c>
       <c r="D24" t="n">
-        <v>0.999225334118937</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.00019366647026594</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.000193666470265788</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
+        <v>0.999473936312373</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25">
@@ -1185,22 +1032,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.987957202874711</v>
+        <v>0.999570319160913</v>
       </c>
       <c r="C25" t="n">
-        <v>0.000158189033636265</v>
+        <v>0.000214840419543665</v>
       </c>
       <c r="D25" t="n">
-        <v>0.000158189033636204</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.000158189033636253</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.0115682300243798</v>
-      </c>
-      <c r="G25" t="s">
-        <v>30</v>
+        <v>0.000214840419543711</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26">
@@ -1208,22 +1049,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.000136580838614994</v>
+        <v>0.000185490085172092</v>
       </c>
       <c r="C26" t="n">
-        <v>0.000136580838615045</v>
+        <v>0.999629019829656</v>
       </c>
       <c r="D26" t="n">
-        <v>0.000136580838615091</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.99945367664554</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.000136580838615033</v>
-      </c>
-      <c r="G26" t="s">
-        <v>31</v>
+        <v>0.00018549008517224</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27">
@@ -1231,22 +1066,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.00011168882954902</v>
+        <v>0.000151680814239032</v>
       </c>
       <c r="C27" t="n">
-        <v>0.000111688829549008</v>
+        <v>0.000151680814239197</v>
       </c>
       <c r="D27" t="n">
-        <v>0.999553244681804</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.000111688829548892</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.000111688829549066</v>
-      </c>
-      <c r="G27" t="s">
-        <v>32</v>
+        <v>0.999696638371522</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28">
@@ -1254,22 +1083,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.999534070044648</v>
+        <v>0.999683616754192</v>
       </c>
       <c r="C28" t="n">
-        <v>0.000116482488838206</v>
+        <v>0.000158191622903831</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000116482488838063</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.000116482488837917</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.000116482488838192</v>
-      </c>
-      <c r="G28" t="s">
-        <v>33</v>
+        <v>0.000158191622903883</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29">
@@ -1277,22 +1100,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.000162241872333957</v>
+        <v>0.000220345506778685</v>
       </c>
       <c r="C29" t="n">
-        <v>0.586269180668495</v>
+        <v>0.999559308986443</v>
       </c>
       <c r="D29" t="n">
-        <v>0.413244093714503</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.000162241872333974</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.000162241872333969</v>
-      </c>
-      <c r="G29" t="s">
-        <v>34</v>
+        <v>0.000220345506778577</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30">
@@ -1300,22 +1117,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.000134644826003831</v>
+        <v>0.999634279073024</v>
       </c>
       <c r="C30" t="n">
-        <v>0.000134644826003759</v>
+        <v>0.00018286046348793</v>
       </c>
       <c r="D30" t="n">
-        <v>0.000134644826003805</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.000134644826003782</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.999461420695985</v>
-      </c>
-      <c r="G30" t="s">
-        <v>35</v>
+        <v>0.000182860463488031</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31">
@@ -1323,22 +1134,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.000201899277272789</v>
+        <v>0.000274215480477308</v>
       </c>
       <c r="C31" t="n">
-        <v>0.000201899277272744</v>
+        <v>0.000274215480477374</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0519201415312905</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.000201899277272732</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0.947474160636891</v>
-      </c>
-      <c r="G31" t="s">
-        <v>36</v>
+        <v>0.999451569039045</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32">
@@ -1346,22 +1151,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.999510036775245</v>
+        <v>0.999667295445671</v>
       </c>
       <c r="C32" t="n">
-        <v>0.000122490806188733</v>
+        <v>0.000166352277164223</v>
       </c>
       <c r="D32" t="n">
-        <v>0.000122490806188688</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.000122490806188747</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.000122490806188775</v>
-      </c>
-      <c r="G32" t="s">
-        <v>37</v>
+        <v>0.000166352277164283</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33">
@@ -1369,22 +1168,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.000186078772847529</v>
+        <v>0.000252724690092138</v>
       </c>
       <c r="C33" t="n">
-        <v>0.000186078772847316</v>
+        <v>0.000252724690092194</v>
       </c>
       <c r="D33" t="n">
-        <v>0.99925568490861</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.000186078772847335</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.000186078772847305</v>
-      </c>
-      <c r="G33" t="s">
-        <v>38</v>
+        <v>0.999494550619816</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34">
@@ -1392,22 +1185,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.000120931357255068</v>
+        <v>0.000164234183979941</v>
       </c>
       <c r="C34" t="n">
-        <v>0.000120931357255171</v>
+        <v>0.000164234183979733</v>
       </c>
       <c r="D34" t="n">
-        <v>0.999516274570979</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.000120931357255154</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.000120931357255211</v>
-      </c>
-      <c r="G34" t="s">
-        <v>39</v>
+        <v>0.99967153163204</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="35">
@@ -1415,22 +1202,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.999382665032685</v>
+        <v>0.999580792591425</v>
       </c>
       <c r="C35" t="n">
-        <v>0.000154333741828916</v>
+        <v>0.000209603704287492</v>
       </c>
       <c r="D35" t="n">
-        <v>0.000154333741828776</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.000154333741828821</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.00015433374182877</v>
-      </c>
-      <c r="G35" t="s">
-        <v>40</v>
+        <v>0.000209603704287457</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="36">
@@ -1438,22 +1219,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.000243264139427258</v>
+        <v>0.00033040905394292</v>
       </c>
       <c r="C36" t="n">
-        <v>0.000243264139427296</v>
+        <v>0.999339181892114</v>
       </c>
       <c r="D36" t="n">
-        <v>0.000243264139427104</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.999026943442291</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.000243264139427214</v>
-      </c>
-      <c r="G36" t="s">
-        <v>41</v>
+        <v>0.000330409053942949</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="37">
@@ -1461,22 +1236,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.000180767041753228</v>
+        <v>0.000245509302912055</v>
       </c>
       <c r="C37" t="n">
-        <v>0.000180767041753158</v>
+        <v>0.000245509302912426</v>
       </c>
       <c r="D37" t="n">
-        <v>0.999276931832987</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.000180767041753072</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.000180767041753189</v>
-      </c>
-      <c r="G37" t="s">
-        <v>42</v>
+        <v>0.999508981394176</v>
+      </c>
+      <c r="E37" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="38">
@@ -1484,22 +1253,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.000104328572326761</v>
+        <v>0.000141684132352576</v>
       </c>
       <c r="C38" t="n">
-        <v>0.000104328572326724</v>
+        <v>0.999716631735295</v>
       </c>
       <c r="D38" t="n">
-        <v>0.000104328572326806</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.999582685710693</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0.000104328572326904</v>
-      </c>
-      <c r="G38" t="s">
-        <v>43</v>
+        <v>0.000141684132352574</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="39">
@@ -1507,22 +1270,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.999441633806337</v>
+        <v>0.99962084109775</v>
       </c>
       <c r="C39" t="n">
-        <v>0.000139591548415682</v>
+        <v>0.0001895794511251</v>
       </c>
       <c r="D39" t="n">
-        <v>0.000139591548415763</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.000139591548415598</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0.000139591548415707</v>
-      </c>
-      <c r="G39" t="s">
-        <v>44</v>
+        <v>0.000189579451125025</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40">
@@ -1530,22 +1287,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.000115071392233927</v>
+        <v>0.999687449904707</v>
       </c>
       <c r="C40" t="n">
-        <v>0.000115071392234121</v>
+        <v>0.000156275047646777</v>
       </c>
       <c r="D40" t="n">
-        <v>0.999539714431064</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.000115071392234307</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0.000115071392234101</v>
-      </c>
-      <c r="G40" t="s">
-        <v>45</v>
+        <v>0.000156275047646634</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="41">
@@ -1553,22 +1304,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.000172557447286781</v>
+        <v>0.000234357635095094</v>
       </c>
       <c r="C41" t="n">
-        <v>0.000172557447287016</v>
+        <v>0.000234357635095063</v>
       </c>
       <c r="D41" t="n">
-        <v>0.999309770210852</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0.000172557447286966</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0.00017255744728684</v>
-      </c>
-      <c r="G41" t="s">
-        <v>46</v>
+        <v>0.99953128472981</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42">
@@ -1576,22 +1321,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>0.450637041914509</v>
+        <v>0.000180304357867206</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0998275801279008</v>
+        <v>0.999639391284265</v>
       </c>
       <c r="D42" t="n">
-        <v>0.000132762931642951</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.449269852094305</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.000132762931643002</v>
-      </c>
-      <c r="G42" t="s">
-        <v>47</v>
+        <v>0.000180304357867468</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="43">
@@ -1599,22 +1338,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>0.000156882711751835</v>
+        <v>0.000213066013808163</v>
       </c>
       <c r="C43" t="n">
-        <v>0.999372469152992</v>
+        <v>0.999573867972383</v>
       </c>
       <c r="D43" t="n">
-        <v>0.000156882711751967</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.000156882711751913</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.000156882711751939</v>
-      </c>
-      <c r="G43" t="s">
-        <v>48</v>
+        <v>0.000213066013808422</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44">
@@ -1622,22 +1355,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>0.638617941977231</v>
+        <v>0.9992841728454</v>
       </c>
       <c r="C44" t="n">
-        <v>0.000263509441713748</v>
+        <v>0.000357913577299953</v>
       </c>
       <c r="D44" t="n">
-        <v>0.360591529697627</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.000263509441713837</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0.000263509441713781</v>
-      </c>
-      <c r="G44" t="s">
-        <v>49</v>
+        <v>0.000357913577300203</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="45">
@@ -1645,22 +1372,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>0.000174139164738624</v>
+        <v>0.999526987640745</v>
       </c>
       <c r="C45" t="n">
-        <v>0.000174139164738656</v>
+        <v>0.000236506179627304</v>
       </c>
       <c r="D45" t="n">
-        <v>0.000174139164738638</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.000174139164738685</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0.999303443341045</v>
-      </c>
-      <c r="G45" t="s">
-        <v>50</v>
+        <v>0.000236506179627287</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="46">
@@ -1668,22 +1389,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>0.000210863117793581</v>
+        <v>0.000286392364069446</v>
       </c>
       <c r="C46" t="n">
-        <v>0.000210863117793591</v>
+        <v>0.000286392364069387</v>
       </c>
       <c r="D46" t="n">
-        <v>0.000210863117793638</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.00021086311779354</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0.999156547528826</v>
-      </c>
-      <c r="G46" t="s">
-        <v>51</v>
+        <v>0.999427215271861</v>
+      </c>
+      <c r="E46" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="47">
@@ -1691,22 +1406,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>0.000163639364804182</v>
+        <v>0.999555512458933</v>
       </c>
       <c r="C47" t="n">
-        <v>0.000163639364804283</v>
+        <v>0.000222243770533535</v>
       </c>
       <c r="D47" t="n">
-        <v>0.000163639364804231</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.000163639364804306</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.999345442540783</v>
-      </c>
-      <c r="G47" t="s">
-        <v>52</v>
+        <v>0.000222243770533596</v>
+      </c>
+      <c r="E47" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="48">
@@ -1714,22 +1423,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>0.00023426490986545</v>
+        <v>0.000318183362759661</v>
       </c>
       <c r="C48" t="n">
-        <v>0.000234264909865385</v>
+        <v>0.0574013859413839</v>
       </c>
       <c r="D48" t="n">
-        <v>0.999062940360538</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0.000234264909865503</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.000234264909865384</v>
-      </c>
-      <c r="G48" t="s">
-        <v>53</v>
+        <v>0.942280430695857</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="49">
@@ -1737,22 +1440,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>0.000130036699902447</v>
+        <v>0.99964679712667</v>
       </c>
       <c r="C49" t="n">
-        <v>0.000130036699902466</v>
+        <v>0.000176601436664941</v>
       </c>
       <c r="D49" t="n">
-        <v>0.000130036699902378</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0.000130036699902473</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0.99947985320039</v>
-      </c>
-      <c r="G49" t="s">
-        <v>54</v>
+        <v>0.000176601436664823</v>
+      </c>
+      <c r="E49" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="50">
@@ -1760,22 +1457,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>0.000179063219129395</v>
+        <v>0.37218316630179</v>
       </c>
       <c r="C50" t="n">
-        <v>0.000179063219129378</v>
+        <v>0.627573638830987</v>
       </c>
       <c r="D50" t="n">
-        <v>0.000179063219129372</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0.000179063219129507</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0.999283747123482</v>
-      </c>
-      <c r="G50" t="s">
-        <v>55</v>
+        <v>0.000243194867222326</v>
+      </c>
+      <c r="E50" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="51">
@@ -1783,22 +1474,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>0.00011941111631766</v>
+        <v>0.000162169350235162</v>
       </c>
       <c r="C51" t="n">
-        <v>0.999522355534729</v>
+        <v>0.000162169350235052</v>
       </c>
       <c r="D51" t="n">
-        <v>0.000119411116317672</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0.000119411116317662</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0.000119411116317749</v>
-      </c>
-      <c r="G51" t="s">
-        <v>56</v>
+        <v>0.99967566129953</v>
+      </c>
+      <c r="E51" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="52">
@@ -1806,22 +1491,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>0.000701152176082292</v>
+        <v>0.000952731228920905</v>
       </c>
       <c r="C52" t="n">
-        <v>0.397630613067648</v>
+        <v>0.000952731228921082</v>
       </c>
       <c r="D52" t="n">
-        <v>0.000701152176082268</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0.000701152176082296</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0.600265930404105</v>
-      </c>
-      <c r="G52" t="s">
-        <v>57</v>
+        <v>0.998094537542158</v>
+      </c>
+      <c r="E52" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="53">
@@ -1829,22 +1508,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0000815020104098802</v>
+        <v>0.999778635953504</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0000815020104100077</v>
+        <v>0.000110682023248224</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0000815020104100332</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0.0000815020104099565</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0.99967399195836</v>
-      </c>
-      <c r="G53" t="s">
-        <v>58</v>
+        <v>0.000110682023248231</v>
+      </c>
+      <c r="E53" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="54">
@@ -1852,22 +1525,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0026776237970034</v>
+        <v>0.247175773360521</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0026776237970034</v>
+        <v>0.749179172671467</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0026776237970034</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0.00267762379700338</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.989289504811986</v>
-      </c>
-      <c r="G54" t="s">
-        <v>59</v>
+        <v>0.00364505396801165</v>
+      </c>
+      <c r="E54" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="55">
@@ -1875,22 +1542,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>0.000412142638074719</v>
+        <v>0.00055987277070474</v>
       </c>
       <c r="C55" t="n">
-        <v>0.998351429447701</v>
+        <v>0.998880254458591</v>
       </c>
       <c r="D55" t="n">
-        <v>0.000412142638074761</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.000412142638074806</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0.000412142638074707</v>
-      </c>
-      <c r="G55" t="s">
-        <v>60</v>
+        <v>0.000559872770704694</v>
+      </c>
+      <c r="E55" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="56">
@@ -1898,22 +1559,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>0.000154333741828714</v>
+        <v>0.000209603704287521</v>
       </c>
       <c r="C56" t="n">
-        <v>0.00015433374182884</v>
+        <v>0.999580792591425</v>
       </c>
       <c r="D56" t="n">
-        <v>0.000154333741828771</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0.999382665032685</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0.000154333741828818</v>
-      </c>
-      <c r="G56" t="s">
-        <v>61</v>
+        <v>0.000209603704287311</v>
+      </c>
+      <c r="E56" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="57">
@@ -1921,22 +1576,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>0.00171227848467063</v>
+        <v>0.0023288402506216</v>
       </c>
       <c r="C57" t="n">
-        <v>0.993150886061318</v>
+        <v>0.995342319498757</v>
       </c>
       <c r="D57" t="n">
-        <v>0.00171227848467064</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0.00171227848467061</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0.00171227848467064</v>
-      </c>
-      <c r="G57" t="s">
-        <v>62</v>
+        <v>0.00232884025062164</v>
+      </c>
+      <c r="E57" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="58">
@@ -1944,22 +1593,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>0.000371811614449697</v>
+        <v>0.000505066451896517</v>
       </c>
       <c r="C58" t="n">
-        <v>0.000371811614449841</v>
+        <v>0.000505066451896538</v>
       </c>
       <c r="D58" t="n">
-        <v>0.000371811614449687</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.998512753542201</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.000371811614449625</v>
-      </c>
-      <c r="G58" t="s">
-        <v>63</v>
+        <v>0.998989867096207</v>
+      </c>
+      <c r="E58" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="59">
@@ -1967,22 +1610,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>0.000106076168502059</v>
+        <v>0.000144057700513881</v>
       </c>
       <c r="C59" t="n">
-        <v>0.999575695325992</v>
+        <v>0.999711884598972</v>
       </c>
       <c r="D59" t="n">
-        <v>0.000106076168502088</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.000106076168502033</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0.000106076168501457</v>
-      </c>
-      <c r="G59" t="s">
-        <v>64</v>
+        <v>0.000144057700513894</v>
+      </c>
+      <c r="E59" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="60">
@@ -1990,22 +1627,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0.000059536222331778</v>
+        <v>0.0000808502199771321</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0000595362223312743</v>
+        <v>0.999838299560046</v>
       </c>
       <c r="D60" t="n">
-        <v>0.000059536222331809</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.0000595362223317675</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0.999761855110673</v>
-      </c>
-      <c r="G60" t="s">
-        <v>65</v>
+        <v>0.0000808502199771222</v>
+      </c>
+      <c r="E60" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="61">
@@ -2013,22 +1644,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>0.000150661897048768</v>
+        <v>0.000204616203350602</v>
       </c>
       <c r="C61" t="n">
-        <v>0.000150661897048864</v>
+        <v>0.999590767593299</v>
       </c>
       <c r="D61" t="n">
-        <v>0.000150661897048862</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.999397352411805</v>
-      </c>
-      <c r="F61" t="n">
-        <v>0.000150661897048928</v>
-      </c>
-      <c r="G61" t="s">
-        <v>66</v>
+        <v>0.000204616203350445</v>
+      </c>
+      <c r="E61" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="62">
@@ -2036,22 +1661,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>0.000100466492152875</v>
+        <v>0.000136438719806324</v>
       </c>
       <c r="C62" t="n">
-        <v>0.999598134031388</v>
+        <v>0.999727122560387</v>
       </c>
       <c r="D62" t="n">
-        <v>0.000100466492153041</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.000100466492152659</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0.000100466492153007</v>
-      </c>
-      <c r="G62" t="s">
-        <v>67</v>
+        <v>0.000136438719806258</v>
+      </c>
+      <c r="E62" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="63">
@@ -2059,22 +1678,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>0.000120931357255104</v>
+        <v>0.000164234183980039</v>
       </c>
       <c r="C63" t="n">
-        <v>0.000120931357255156</v>
+        <v>0.000164234183979822</v>
       </c>
       <c r="D63" t="n">
-        <v>0.000120931357255123</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.999516274570979</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0.000120931357255132</v>
-      </c>
-      <c r="G63" t="s">
-        <v>65</v>
+        <v>0.99967153163204</v>
+      </c>
+      <c r="E63" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="64">
@@ -2082,22 +1695,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>0.99962583596338</v>
+        <v>0.999745934522215</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0000935410091549534</v>
+        <v>0.000127032738892426</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0000935410091552162</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0.0000935410091546553</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0.0000935410091551701</v>
-      </c>
-      <c r="G64" t="s">
-        <v>68</v>
+        <v>0.000127032738892213</v>
+      </c>
+      <c r="E64" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="65">
@@ -2105,22 +1712,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0026776237970034</v>
+        <v>0.00364505396801167</v>
       </c>
       <c r="C65" t="n">
-        <v>0.989289504811986</v>
+        <v>0.992709892063977</v>
       </c>
       <c r="D65" t="n">
-        <v>0.00267762379700339</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0.00267762379700338</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0.00267762379700336</v>
-      </c>
-      <c r="G65" t="s">
-        <v>69</v>
+        <v>0.00364505396801166</v>
+      </c>
+      <c r="E65" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="66">
@@ -2128,22 +1729,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>0.873093391356032</v>
+        <v>0.767295259441872</v>
       </c>
       <c r="C66" t="n">
-        <v>0.125791173800619</v>
+        <v>0.232199674106232</v>
       </c>
       <c r="D66" t="n">
-        <v>0.000371811614449597</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.000371811614449722</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0.000371811614449627</v>
-      </c>
-      <c r="G66" t="s">
-        <v>70</v>
+        <v>0.000505066451896547</v>
+      </c>
+      <c r="E66" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="67">
@@ -2151,22 +1746,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>0.000557199488570846</v>
+        <v>0.000757026155073745</v>
       </c>
       <c r="C67" t="n">
-        <v>0.997771202045717</v>
+        <v>0.657721913705605</v>
       </c>
       <c r="D67" t="n">
-        <v>0.000557199488570825</v>
-      </c>
-      <c r="E67" t="n">
-        <v>0.000557199488570796</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0.000557199488570812</v>
-      </c>
-      <c r="G67" t="s">
-        <v>68</v>
+        <v>0.341521060139321</v>
+      </c>
+      <c r="E67" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="68">
@@ -2174,22 +1763,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>0.00038695823635235</v>
+        <v>0.000525648900428026</v>
       </c>
       <c r="C68" t="n">
-        <v>0.000386958236352498</v>
+        <v>0.998948702199144</v>
       </c>
       <c r="D68" t="n">
-        <v>0.000386958236352315</v>
-      </c>
-      <c r="E68" t="n">
-        <v>0.998452167054591</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0.000386958236352322</v>
-      </c>
-      <c r="G68" t="s">
-        <v>68</v>
+        <v>0.000525648900428076</v>
+      </c>
+      <c r="E68" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="69">
@@ -2197,22 +1780,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>0.000180767041753141</v>
+        <v>0.000245509302911915</v>
       </c>
       <c r="C69" t="n">
-        <v>0.162374128291525</v>
+        <v>0.000245509302912009</v>
       </c>
       <c r="D69" t="n">
-        <v>0.837083570583215</v>
-      </c>
-      <c r="E69" t="n">
-        <v>0.000180767041753239</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0.000180767041753211</v>
-      </c>
-      <c r="G69" t="s">
-        <v>68</v>
+        <v>0.999508981394176</v>
+      </c>
+      <c r="E69" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="70">
@@ -2220,22 +1797,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>0.00118034940648151</v>
+        <v>0.00160458093417572</v>
       </c>
       <c r="C70" t="n">
-        <v>0.995278602374074</v>
+        <v>0.996790838131649</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00118034940648152</v>
-      </c>
-      <c r="E70" t="n">
-        <v>0.0011803494064815</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0.00118034940648152</v>
-      </c>
-      <c r="G70" t="s">
-        <v>71</v>
+        <v>0.0016045809341757</v>
+      </c>
+      <c r="E70" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="71">
@@ -2243,22 +1814,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>0.0023468483079263</v>
+        <v>0.00319378779533883</v>
       </c>
       <c r="C71" t="n">
-        <v>0.990612606768295</v>
+        <v>0.993612424409322</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00234684830792629</v>
-      </c>
-      <c r="E71" t="n">
-        <v>0.00234684830792627</v>
-      </c>
-      <c r="F71" t="n">
-        <v>0.00234684830792627</v>
-      </c>
-      <c r="G71" t="s">
-        <v>72</v>
+        <v>0.00319378779533886</v>
+      </c>
+      <c r="E71" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="72">
@@ -2266,22 +1831,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>0.000332738663507427</v>
+        <v>0.000451973649610861</v>
       </c>
       <c r="C72" t="n">
-        <v>0.99866904534597</v>
+        <v>0.999096052700778</v>
       </c>
       <c r="D72" t="n">
-        <v>0.000332738663507422</v>
-      </c>
-      <c r="E72" t="n">
-        <v>0.000332738663507413</v>
-      </c>
-      <c r="F72" t="n">
-        <v>0.00033273866350744</v>
-      </c>
-      <c r="G72" t="s">
-        <v>71</v>
+        <v>0.000451973649610977</v>
+      </c>
+      <c r="E72" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="73">
@@ -2289,22 +1848,16 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>0.00049869315902293</v>
+        <v>0.000677501155411522</v>
       </c>
       <c r="C73" t="n">
-        <v>0.998005227363908</v>
+        <v>0.998644997689177</v>
       </c>
       <c r="D73" t="n">
-        <v>0.000498693159022927</v>
-      </c>
-      <c r="E73" t="n">
-        <v>0.000498693159022892</v>
-      </c>
-      <c r="F73" t="n">
-        <v>0.000498693159022909</v>
-      </c>
-      <c r="G73" t="s">
-        <v>71</v>
+        <v>0.000677501155411564</v>
+      </c>
+      <c r="E73" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="74">
@@ -2312,22 +1865,16 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>0.000104904670943121</v>
+        <v>0.00014246658305208</v>
       </c>
       <c r="C74" t="n">
-        <v>0.000104904670943235</v>
+        <v>0.00014246658305184</v>
       </c>
       <c r="D74" t="n">
-        <v>0.999580381316227</v>
-      </c>
-      <c r="E74" t="n">
-        <v>0.000104904670942994</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0.000104904670943307</v>
-      </c>
-      <c r="G74" t="s">
-        <v>73</v>
+        <v>0.999715066833896</v>
+      </c>
+      <c r="E74" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="75">
@@ -2335,22 +1882,16 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>0.597360992378247</v>
+        <v>0.575975275528915</v>
       </c>
       <c r="C75" t="n">
-        <v>0.000160868047124964</v>
+        <v>0.000218479395898189</v>
       </c>
       <c r="D75" t="n">
-        <v>0.402156403480378</v>
-      </c>
-      <c r="E75" t="n">
-        <v>0.000160868047125163</v>
-      </c>
-      <c r="F75" t="n">
-        <v>0.000160868047125121</v>
-      </c>
-      <c r="G75" t="s">
-        <v>74</v>
+        <v>0.423806245075186</v>
+      </c>
+      <c r="E75" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="76">
@@ -2358,22 +1899,16 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>0.000158189033636261</v>
+        <v>0.000214840419543655</v>
       </c>
       <c r="C76" t="n">
-        <v>0.999367243865455</v>
+        <v>0.999570319160913</v>
       </c>
       <c r="D76" t="n">
-        <v>0.000158189033636242</v>
-      </c>
-      <c r="E76" t="n">
-        <v>0.00015818903363627</v>
-      </c>
-      <c r="F76" t="n">
-        <v>0.000158189033636358</v>
-      </c>
-      <c r="G76" t="s">
-        <v>75</v>
+        <v>0.000214840419543443</v>
+      </c>
+      <c r="E76" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="77">
@@ -2381,22 +1916,16 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>0.000167980123848593</v>
+        <v>0.000228140009359438</v>
       </c>
       <c r="C77" t="n">
-        <v>0.999328079504606</v>
+        <v>0.999543719981281</v>
       </c>
       <c r="D77" t="n">
-        <v>0.000167980123848516</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0.000167980123848666</v>
-      </c>
-      <c r="F77" t="n">
-        <v>0.000167980123848549</v>
-      </c>
-      <c r="G77" t="s">
-        <v>76</v>
+        <v>0.000228140009359095</v>
+      </c>
+      <c r="E77" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="78">
@@ -2404,22 +1933,16 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>0.000274950623508851</v>
+        <v>0.000373457602545923</v>
       </c>
       <c r="C78" t="n">
-        <v>0.000274950623508914</v>
+        <v>0.999253084794908</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00027495062350895</v>
-      </c>
-      <c r="E78" t="n">
-        <v>0.998900197505964</v>
-      </c>
-      <c r="F78" t="n">
-        <v>0.000274950623508842</v>
-      </c>
-      <c r="G78" t="s">
-        <v>77</v>
+        <v>0.000373457602545935</v>
+      </c>
+      <c r="E78" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="79">
@@ -2427,22 +1950,16 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>0.000139591548415794</v>
+        <v>0.000189579451124942</v>
       </c>
       <c r="C79" t="n">
-        <v>0.000139591548415636</v>
+        <v>0.000189579451124988</v>
       </c>
       <c r="D79" t="n">
-        <v>0.999441633806337</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0.000139591548415699</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0.000139591548415712</v>
-      </c>
-      <c r="G79" t="s">
-        <v>78</v>
+        <v>0.99962084109775</v>
+      </c>
+      <c r="E79" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="80">
@@ -2450,22 +1967,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>0.999345442540783</v>
+        <v>0.000222243770533218</v>
       </c>
       <c r="C80" t="n">
-        <v>0.000163639364804314</v>
+        <v>0.000222243770533573</v>
       </c>
       <c r="D80" t="n">
-        <v>0.000163639364804232</v>
-      </c>
-      <c r="E80" t="n">
-        <v>0.000163639364804326</v>
-      </c>
-      <c r="F80" t="n">
-        <v>0.000163639364804292</v>
-      </c>
-      <c r="G80" t="s">
-        <v>79</v>
+        <v>0.999555512458933</v>
+      </c>
+      <c r="E80" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="81">
@@ -2473,22 +1984,16 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>0.000151866277006868</v>
+        <v>0.000206252120116684</v>
       </c>
       <c r="C81" t="n">
-        <v>0.000151866277006841</v>
+        <v>0.000206252120116876</v>
       </c>
       <c r="D81" t="n">
-        <v>0.999392534891973</v>
-      </c>
-      <c r="E81" t="n">
-        <v>0.00015186627700684</v>
-      </c>
-      <c r="F81" t="n">
-        <v>0.000151866277006777</v>
-      </c>
-      <c r="G81" t="s">
-        <v>80</v>
+        <v>0.999587495759766</v>
+      </c>
+      <c r="E81" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="82">
@@ -2496,22 +2001,16 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>0.000231411326303149</v>
+        <v>0.000314306736646838</v>
       </c>
       <c r="C82" t="n">
-        <v>0.000231411326303229</v>
+        <v>0.183744984061992</v>
       </c>
       <c r="D82" t="n">
-        <v>0.000231411326303201</v>
-      </c>
-      <c r="E82" t="n">
-        <v>0.999074354694787</v>
-      </c>
-      <c r="F82" t="n">
-        <v>0.00023141132630315</v>
-      </c>
-      <c r="G82" t="s">
-        <v>81</v>
+        <v>0.815940709201361</v>
+      </c>
+      <c r="E82" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="83">
@@ -2519,22 +2018,16 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>0.000512136839112977</v>
+        <v>0.000695773776838653</v>
       </c>
       <c r="C83" t="n">
-        <v>0.000512136839113001</v>
+        <v>0.998608452446323</v>
       </c>
       <c r="D83" t="n">
-        <v>0.000512136839112987</v>
-      </c>
-      <c r="E83" t="n">
-        <v>0.997951452643548</v>
-      </c>
-      <c r="F83" t="n">
-        <v>0.00051213683911299</v>
-      </c>
-      <c r="G83" t="s">
-        <v>82</v>
+        <v>0.000695773776838578</v>
+      </c>
+      <c r="E83" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="84">
@@ -2542,22 +2035,16 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>0.000116482488838033</v>
+        <v>0.00022034550677883</v>
       </c>
       <c r="C84" t="n">
-        <v>0.00011648248883814</v>
+        <v>0.000220345506778711</v>
       </c>
       <c r="D84" t="n">
-        <v>0.000116482488837634</v>
-      </c>
-      <c r="E84" t="n">
-        <v>0.999534070044648</v>
-      </c>
-      <c r="F84" t="n">
-        <v>0.000116482488838154</v>
-      </c>
-      <c r="G84" t="s">
-        <v>83</v>
+        <v>0.999559308986442</v>
+      </c>
+      <c r="E84" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="85">
@@ -2565,22 +2052,16 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>0.000162241872333917</v>
+        <v>0.00032623075413087</v>
       </c>
       <c r="C85" t="n">
-        <v>0.000162241872334001</v>
+        <v>0.000326230754130997</v>
       </c>
       <c r="D85" t="n">
-        <v>0.000162241872333895</v>
-      </c>
-      <c r="E85" t="n">
-        <v>0.999351032510664</v>
-      </c>
-      <c r="F85" t="n">
-        <v>0.000162241872333988</v>
-      </c>
-      <c r="G85" t="s">
-        <v>84</v>
+        <v>0.999347538491738</v>
+      </c>
+      <c r="E85" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="86">
@@ -2588,22 +2069,16 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>0.000240188544577478</v>
+        <v>0.000163195236022549</v>
       </c>
       <c r="C86" t="n">
-        <v>0.000240188544577499</v>
+        <v>0.999673609527955</v>
       </c>
       <c r="D86" t="n">
-        <v>0.99903924582169</v>
-      </c>
-      <c r="E86" t="n">
-        <v>0.000240188544577626</v>
-      </c>
-      <c r="F86" t="n">
-        <v>0.000240188544577493</v>
-      </c>
-      <c r="G86" t="s">
-        <v>85</v>
+        <v>0.000163195236022319</v>
+      </c>
+      <c r="E86" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="87">
@@ -2611,22 +2086,16 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>0.000120166428787629</v>
+        <v>0.000157227494814663</v>
       </c>
       <c r="C87" t="n">
-        <v>0.999519334284849</v>
+        <v>0.999685545010371</v>
       </c>
       <c r="D87" t="n">
-        <v>0.0001201664287879</v>
-      </c>
-      <c r="E87" t="n">
-        <v>0.000120166428787641</v>
-      </c>
-      <c r="F87" t="n">
-        <v>0.000120166428787995</v>
-      </c>
-      <c r="G87" t="s">
-        <v>86</v>
+        <v>0.000157227494814157</v>
+      </c>
+      <c r="E87" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="88">
@@ -2634,22 +2103,16 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>0.000115772640902516</v>
+        <v>0.000408981354065682</v>
       </c>
       <c r="C88" t="n">
-        <v>0.000115772640902552</v>
+        <v>0.999182037291868</v>
       </c>
       <c r="D88" t="n">
-        <v>0.000115772640902524</v>
-      </c>
-      <c r="E88" t="n">
-        <v>0.99953690943639</v>
-      </c>
-      <c r="F88" t="n">
-        <v>0.000115772640902554</v>
-      </c>
-      <c r="G88" t="s">
-        <v>87</v>
+        <v>0.00040898135406583</v>
+      </c>
+      <c r="E88" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="89">
@@ -2657,22 +2120,16 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>0.000301096974890096</v>
+        <v>0.000243194867222403</v>
       </c>
       <c r="C89" t="n">
-        <v>0.998795612100439</v>
+        <v>0.000243194867222377</v>
       </c>
       <c r="D89" t="n">
-        <v>0.000301096974890235</v>
-      </c>
-      <c r="E89" t="n">
-        <v>0.000301096974890151</v>
-      </c>
-      <c r="F89" t="n">
-        <v>0.000301096974890152</v>
-      </c>
-      <c r="G89" t="s">
-        <v>88</v>
+        <v>0.999513610265555</v>
+      </c>
+      <c r="E89" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="90">
@@ -2680,22 +2137,16 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>0.000179063219129384</v>
+        <v>0.00015257792302507</v>
       </c>
       <c r="C90" t="n">
-        <v>0.000179063219129321</v>
+        <v>0.000152577923025039</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2200203292023</v>
-      </c>
-      <c r="E90" t="n">
-        <v>0.779442481140311</v>
-      </c>
-      <c r="F90" t="n">
-        <v>0.000179063219129393</v>
-      </c>
-      <c r="G90" t="s">
-        <v>89</v>
+        <v>0.99969484415395</v>
+      </c>
+      <c r="E90" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="91">
@@ -2703,22 +2154,16 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>0.000112349338949871</v>
+        <v>0.000559872770704766</v>
       </c>
       <c r="C91" t="n">
-        <v>0.000112349338949943</v>
+        <v>0.000559872770704764</v>
       </c>
       <c r="D91" t="n">
-        <v>0.9995506026442</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0.000112349338949821</v>
-      </c>
-      <c r="F91" t="n">
-        <v>0.000112349338949863</v>
-      </c>
-      <c r="G91" t="s">
-        <v>90</v>
+        <v>0.99888025445859</v>
+      </c>
+      <c r="E91" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="92">
@@ -2726,22 +2171,16 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>0.000412142638074751</v>
+        <v>0.999634279073024</v>
       </c>
       <c r="C92" t="n">
-        <v>0.0456559592322562</v>
+        <v>0.000182860463487776</v>
       </c>
       <c r="D92" t="n">
-        <v>0.95310761285352</v>
-      </c>
-      <c r="E92" t="n">
-        <v>0.000412142638074702</v>
-      </c>
-      <c r="F92" t="n">
-        <v>0.000412142638074731</v>
-      </c>
-      <c r="G92" t="s">
-        <v>91</v>
+        <v>0.000182860463487691</v>
+      </c>
+      <c r="E92" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="93">
@@ -2749,45 +2188,16 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>0.999461420695986</v>
+        <v>0.000149917877085558</v>
       </c>
       <c r="C93" t="n">
-        <v>0.000134644826003565</v>
+        <v>0.703848046090835</v>
       </c>
       <c r="D93" t="n">
-        <v>0.000134644826003503</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.000134644826003613</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0.00013464482600366</v>
-      </c>
-      <c r="G93" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>93</v>
-      </c>
-      <c r="B94" t="n">
-        <v>0.000110390839055501</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0.000110390839055701</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0.000110390839055702</v>
-      </c>
-      <c r="E94" t="n">
-        <v>0.999558436643777</v>
-      </c>
-      <c r="F94" t="n">
-        <v>0.00011039083905567</v>
-      </c>
-      <c r="G94" t="s">
-        <v>93</v>
+        <v>0.296002036032079</v>
+      </c>
+      <c r="E93" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>